<commit_message>
Enhanced table headers with bold styling and improved tab navigation with bigger fonts, hover effects, and active tab highlighting
</commit_message>
<xml_diff>
--- a/summary_reports.xlsx
+++ b/summary_reports.xlsx
@@ -468,10 +468,10 @@
         <v>1077</v>
       </c>
       <c r="C2" t="n">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="D2" t="n">
-        <v>14.95</v>
+        <v>16.71</v>
       </c>
     </row>
     <row r="3">
@@ -500,10 +500,10 @@
         <v>429</v>
       </c>
       <c r="C4" t="n">
-        <v>216</v>
+        <v>243</v>
       </c>
       <c r="D4" t="n">
-        <v>50.35</v>
+        <v>56.64</v>
       </c>
     </row>
     <row r="5">
@@ -516,10 +516,10 @@
         <v>274</v>
       </c>
       <c r="C5" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D5" t="n">
-        <v>46.35</v>
+        <v>46.72</v>
       </c>
     </row>
     <row r="6">
@@ -532,10 +532,10 @@
         <v>300</v>
       </c>
       <c r="C6" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D6" t="n">
-        <v>30.33</v>
+        <v>30.67</v>
       </c>
     </row>
     <row r="7">
@@ -548,10 +548,10 @@
         <v>838</v>
       </c>
       <c r="C7" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D7" t="n">
-        <v>10.86</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="8">
@@ -580,10 +580,10 @@
         <v>330</v>
       </c>
       <c r="C9" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D9" t="n">
-        <v>29.39</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="10">
@@ -596,10 +596,10 @@
         <v>625</v>
       </c>
       <c r="C10" t="n">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D10" t="n">
-        <v>24.48</v>
+        <v>25.12</v>
       </c>
     </row>
     <row r="11">
@@ -644,10 +644,10 @@
         <v>354</v>
       </c>
       <c r="C13" t="n">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D13" t="n">
-        <v>38.14</v>
+        <v>39.83</v>
       </c>
     </row>
     <row r="14">
@@ -660,10 +660,10 @@
         <v>529</v>
       </c>
       <c r="C14" t="n">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D14" t="n">
-        <v>41.21</v>
+        <v>41.59</v>
       </c>
     </row>
     <row r="15">
@@ -676,10 +676,10 @@
         <v>442</v>
       </c>
       <c r="C15" t="n">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D15" t="n">
-        <v>28.51</v>
+        <v>29.86</v>
       </c>
     </row>
     <row r="16">
@@ -692,10 +692,10 @@
         <v>231</v>
       </c>
       <c r="C16" t="n">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D16" t="n">
-        <v>47.19</v>
+        <v>53.25</v>
       </c>
     </row>
     <row r="17">
@@ -724,10 +724,10 @@
         <v>324</v>
       </c>
       <c r="C18" t="n">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D18" t="n">
-        <v>22.22</v>
+        <v>25.62</v>
       </c>
     </row>
     <row r="19">
@@ -756,10 +756,10 @@
         <v>290</v>
       </c>
       <c r="C20" t="n">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D20" t="n">
-        <v>64.48</v>
+        <v>66.20999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -852,10 +852,10 @@
         <v>323</v>
       </c>
       <c r="C26" t="n">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="D26" t="n">
-        <v>27.24</v>
+        <v>34.37</v>
       </c>
     </row>
     <row r="27">
@@ -868,10 +868,10 @@
         <v>463</v>
       </c>
       <c r="C27" t="n">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="D27" t="n">
-        <v>51.4</v>
+        <v>54.21</v>
       </c>
     </row>
     <row r="28">
@@ -884,10 +884,10 @@
         <v>614</v>
       </c>
       <c r="C28" t="n">
-        <v>159</v>
+        <v>243</v>
       </c>
       <c r="D28" t="n">
-        <v>25.9</v>
+        <v>39.58</v>
       </c>
     </row>
     <row r="29">
@@ -900,10 +900,10 @@
         <v>389</v>
       </c>
       <c r="C29" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D29" t="n">
-        <v>39.07</v>
+        <v>39.33</v>
       </c>
     </row>
     <row r="30">
@@ -948,10 +948,10 @@
         <v>540</v>
       </c>
       <c r="C32" t="n">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="D32" t="n">
-        <v>19.07</v>
+        <v>21.11</v>
       </c>
     </row>
     <row r="33">
@@ -964,10 +964,10 @@
         <v>686</v>
       </c>
       <c r="C33" t="n">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="D33" t="n">
-        <v>41.55</v>
+        <v>43.15</v>
       </c>
     </row>
     <row r="34">
@@ -996,10 +996,10 @@
         <v>163</v>
       </c>
       <c r="C35" t="n">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D35" t="n">
-        <v>72.39</v>
+        <v>74.84999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1012,10 +1012,10 @@
         <v>631</v>
       </c>
       <c r="C36" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D36" t="n">
-        <v>26.15</v>
+        <v>26.47</v>
       </c>
     </row>
     <row r="37">
@@ -1028,10 +1028,10 @@
         <v>385</v>
       </c>
       <c r="C37" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D37" t="n">
-        <v>22.6</v>
+        <v>23.12</v>
       </c>
     </row>
     <row r="38">
@@ -1060,10 +1060,10 @@
         <v>828</v>
       </c>
       <c r="C39" t="n">
-        <v>267</v>
+        <v>299</v>
       </c>
       <c r="D39" t="n">
-        <v>32.25</v>
+        <v>36.11</v>
       </c>
     </row>
     <row r="40">
@@ -1076,10 +1076,10 @@
         <v>300</v>
       </c>
       <c r="C40" t="n">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="D40" t="n">
-        <v>59.33</v>
+        <v>63.67</v>
       </c>
     </row>
     <row r="41">
@@ -1092,10 +1092,10 @@
         <v>406</v>
       </c>
       <c r="C41" t="n">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="D41" t="n">
-        <v>41.87</v>
+        <v>46.31</v>
       </c>
     </row>
     <row r="42">
@@ -1108,10 +1108,10 @@
         <v>385</v>
       </c>
       <c r="C42" t="n">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D42" t="n">
-        <v>31.17</v>
+        <v>32.73</v>
       </c>
     </row>
     <row r="43">
@@ -1140,10 +1140,10 @@
         <v>873</v>
       </c>
       <c r="C44" t="n">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D44" t="n">
-        <v>36.2</v>
+        <v>36.66</v>
       </c>
     </row>
     <row r="45">
@@ -1172,10 +1172,10 @@
         <v>361</v>
       </c>
       <c r="C46" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D46" t="n">
-        <v>24.93</v>
+        <v>25.21</v>
       </c>
     </row>
     <row r="47">
@@ -1188,10 +1188,10 @@
         <v>365</v>
       </c>
       <c r="C47" t="n">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="D47" t="n">
-        <v>67.12</v>
+        <v>69.86</v>
       </c>
     </row>
     <row r="48">
@@ -1236,10 +1236,10 @@
         <v>1051</v>
       </c>
       <c r="C50" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D50" t="n">
-        <v>28.54</v>
+        <v>28.64</v>
       </c>
     </row>
     <row r="51">
@@ -1252,10 +1252,10 @@
         <v>320</v>
       </c>
       <c r="C51" t="n">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="D51" t="n">
-        <v>52.19</v>
+        <v>55.94</v>
       </c>
     </row>
     <row r="52">
@@ -1268,10 +1268,10 @@
         <v>112</v>
       </c>
       <c r="C52" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D52" t="n">
-        <v>64.29000000000001</v>
+        <v>69.64</v>
       </c>
     </row>
     <row r="53">
@@ -1316,10 +1316,10 @@
         <v>522</v>
       </c>
       <c r="C55" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D55" t="n">
-        <v>11.49</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="56">
@@ -1332,10 +1332,10 @@
         <v>572</v>
       </c>
       <c r="C56" t="n">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="D56" t="n">
-        <v>48.25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57">
@@ -1348,10 +1348,10 @@
         <v>347</v>
       </c>
       <c r="C57" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D57" t="n">
-        <v>40.35</v>
+        <v>41.21</v>
       </c>
     </row>
     <row r="58">
@@ -1364,10 +1364,10 @@
         <v>537</v>
       </c>
       <c r="C58" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D58" t="n">
-        <v>37.8</v>
+        <v>38.18</v>
       </c>
     </row>
     <row r="59">
@@ -1380,10 +1380,10 @@
         <v>388</v>
       </c>
       <c r="C59" t="n">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D59" t="n">
-        <v>44.33</v>
+        <v>46.39</v>
       </c>
     </row>
     <row r="60">
@@ -1396,10 +1396,10 @@
         <v>225</v>
       </c>
       <c r="C60" t="n">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D60" t="n">
-        <v>56</v>
+        <v>60.44</v>
       </c>
     </row>
     <row r="61">
@@ -1412,10 +1412,10 @@
         <v>742</v>
       </c>
       <c r="C61" t="n">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D61" t="n">
-        <v>30.59</v>
+        <v>31.81</v>
       </c>
     </row>
     <row r="62">
@@ -1460,10 +1460,10 @@
         <v>266</v>
       </c>
       <c r="C64" t="n">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D64" t="n">
-        <v>62.41</v>
+        <v>64.66</v>
       </c>
     </row>
     <row r="65">
@@ -1476,10 +1476,10 @@
         <v>452</v>
       </c>
       <c r="C65" t="n">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="D65" t="n">
-        <v>51.99</v>
+        <v>58.63</v>
       </c>
     </row>
     <row r="66">
@@ -1508,10 +1508,10 @@
         <v>310</v>
       </c>
       <c r="C67" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D67" t="n">
-        <v>19.68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68">
@@ -1540,10 +1540,10 @@
         <v>150</v>
       </c>
       <c r="C69" t="n">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D69" t="n">
-        <v>75.33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70">
@@ -1588,10 +1588,10 @@
         <v>468</v>
       </c>
       <c r="C72" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D72" t="n">
-        <v>35.26</v>
+        <v>35.47</v>
       </c>
     </row>
     <row r="73">
@@ -1604,10 +1604,10 @@
         <v>239</v>
       </c>
       <c r="C73" t="n">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D73" t="n">
-        <v>32.22</v>
+        <v>34.31</v>
       </c>
     </row>
     <row r="74">
@@ -1620,10 +1620,10 @@
         <v>395</v>
       </c>
       <c r="C74" t="n">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D74" t="n">
-        <v>54.18</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="75">
@@ -1636,10 +1636,10 @@
         <v>435</v>
       </c>
       <c r="C75" t="n">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D75" t="n">
-        <v>85.98</v>
+        <v>86.90000000000001</v>
       </c>
     </row>
     <row r="76">
@@ -1652,10 +1652,10 @@
         <v>622</v>
       </c>
       <c r="C76" t="n">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D76" t="n">
-        <v>34.24</v>
+        <v>36.66</v>
       </c>
     </row>
     <row r="77">
@@ -1668,10 +1668,10 @@
         <v>33332</v>
       </c>
       <c r="C77" t="n">
-        <v>11209</v>
+        <v>11687</v>
       </c>
       <c r="D77" t="n">
-        <v>33.63</v>
+        <v>35.06</v>
       </c>
     </row>
   </sheetData>
@@ -1725,10 +1725,10 @@
         <v>435</v>
       </c>
       <c r="C2" t="n">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D2" t="n">
-        <v>85.98</v>
+        <v>86.90000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -1741,10 +1741,10 @@
         <v>150</v>
       </c>
       <c r="C3" t="n">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D3" t="n">
-        <v>75.33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
@@ -1757,10 +1757,10 @@
         <v>163</v>
       </c>
       <c r="C4" t="n">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D4" t="n">
-        <v>72.39</v>
+        <v>74.84999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -1773,26 +1773,26 @@
         <v>365</v>
       </c>
       <c r="C5" t="n">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="D5" t="n">
-        <v>67.12</v>
+        <v>69.86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SHRAWASTI</t>
+          <t>MAHOBA</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="C6" t="n">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D6" t="n">
-        <v>65.38</v>
+        <v>69.64</v>
       </c>
     </row>
     <row r="7">
@@ -1805,74 +1805,74 @@
         <v>290</v>
       </c>
       <c r="C7" t="n">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D7" t="n">
-        <v>64.48</v>
+        <v>66.20999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MAHOBA</t>
+          <t>SHRAWASTI</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C8" t="n">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D8" t="n">
-        <v>64.29000000000001</v>
+        <v>65.38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CHITRAKOOT</t>
+          <t>RAMPUR</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>134</v>
+        <v>266</v>
       </c>
       <c r="C9" t="n">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="D9" t="n">
-        <v>63.43</v>
+        <v>64.66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RAMPUR</t>
+          <t>JHANSI</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="C10" t="n">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="D10" t="n">
-        <v>62.41</v>
+        <v>63.67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SAMBHAL (BHIM NAGAR)</t>
+          <t>CHITRAKOOT</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>262</v>
+        <v>134</v>
       </c>
       <c r="C11" t="n">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="D11" t="n">
-        <v>59.54</v>
+        <v>63.43</v>
       </c>
     </row>
   </sheetData>
@@ -1958,10 +1958,10 @@
         <v>838</v>
       </c>
       <c r="C4" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D4" t="n">
-        <v>10.86</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="5">
@@ -1974,42 +1974,42 @@
         <v>522</v>
       </c>
       <c r="C5" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" t="n">
-        <v>11.49</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AGRA</t>
+          <t>PRAYAGRAJ</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1077</v>
+        <v>1181</v>
       </c>
       <c r="C6" t="n">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="D6" t="n">
-        <v>14.95</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PRAYAGRAJ</t>
+          <t>AGRA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1181</v>
+        <v>1077</v>
       </c>
       <c r="C7" t="n">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D7" t="n">
-        <v>15.5</v>
+        <v>16.71</v>
       </c>
     </row>
     <row r="8">
@@ -2047,33 +2047,33 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GONDA</t>
+          <t>DEORIA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>540</v>
+        <v>580</v>
       </c>
       <c r="C10" t="n">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D10" t="n">
-        <v>19.07</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DEORIA</t>
+          <t>SANT KABIR NAGAR</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>580</v>
+        <v>310</v>
       </c>
       <c r="C11" t="n">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="D11" t="n">
-        <v>19.31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2124,7 +2124,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11209</v>
+        <v>11687</v>
       </c>
     </row>
     <row r="4">
@@ -2134,7 +2134,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.63</v>
+        <v>35.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>